<commit_message>
Db structrue changed + working state machine
</commit_message>
<xml_diff>
--- a/Others/Documentation/Price Estimation.xlsx
+++ b/Others/Documentation/Price Estimation.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\Monitor\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\Monitor\Others\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="State function" sheetId="2" r:id="rId2"/>
+    <sheet name="Lamda function" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Price Calculation</t>
   </si>
@@ -51,13 +53,46 @@
   </si>
   <si>
     <t>Amazon AuroraL woth MySQL DB</t>
+  </si>
+  <si>
+    <t>Step function 10k sites</t>
+  </si>
+  <si>
+    <t>Invocation amout for each site</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/lambda/pricing/</t>
+  </si>
+  <si>
+    <t>Calculator link</t>
+  </si>
+  <si>
+    <t>Calculation invocation amount (based on periodicy of 5m, 1h, 1w, 1m)</t>
+  </si>
+  <si>
+    <t>5m in month</t>
+  </si>
+  <si>
+    <t>1d in month</t>
+  </si>
+  <si>
+    <t>1w in month</t>
+  </si>
+  <si>
+    <t>1m in month</t>
+  </si>
+  <si>
+    <t>Total month invocation per site</t>
+  </si>
+  <si>
+    <t>Total month invocation 10k res</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +110,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,24 +171,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,6 +211,92 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>141943</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="7457143" cy="4028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>303771</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>8714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="8228571" cy="6485714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:G23"/>
+  <dimension ref="C3:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,26 +573,31 @@
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E3" s="2" t="s">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="3" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>1</v>
       </c>
@@ -461,7 +608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
@@ -476,7 +623,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -494,14 +641,14 @@
         <v>15.33</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="3" t="s">
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>1</v>
       </c>
@@ -512,7 +659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
@@ -524,7 +671,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
@@ -539,11 +686,11 @@
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
@@ -583,7 +730,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="J6:L6"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="C22:D22"/>
@@ -597,4 +745,120 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="O4:R4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O4" sqref="O4:R4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="O4:Q4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="O3:Q12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="16" max="16" width="19.140625" customWidth="1"/>
+    <col min="17" max="17" width="39.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5">
+        <f>43800/5</f>
+        <v>8760</v>
+      </c>
+    </row>
+    <row r="6" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6">
+        <f>43800/1440</f>
+        <v>30.416666666666668</v>
+      </c>
+    </row>
+    <row r="7" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="5">
+        <f>43800/10080</f>
+        <v>4.3452380952380949</v>
+      </c>
+    </row>
+    <row r="8" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q8">
+        <f>43800/43800</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11">
+        <f>Q5+Q6+Q7+Q8</f>
+        <v>8795.7619047619046</v>
+      </c>
+    </row>
+    <row r="12" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>